<commit_message>
resultat confort et restau choisis
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/testToursParole.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/testToursParole.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Normalité Test" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="tourParole" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="diffTour" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="calculTour" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t xml:space="preserve">Normalité</t>
   </si>
@@ -205,16 +206,23 @@
   </si>
   <si>
     <t xml:space="preserve">0.06986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilcox (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne pas prendre en compte !!!!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -270,6 +278,25 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="'Ubuntu Mono'"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -309,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -322,6 +349,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -350,7 +384,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,12 +405,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -409,6 +443,50 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -490,13 +568,13 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,18 +725,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -671,945 +749,1255 @@
       <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="F2" s="0" t="n">
+        <f aca="false">ABS(C2-B2)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="6" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="F3" s="0" t="n">
+        <f aca="false">ABS(C3-B3)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="F4" s="0" t="n">
+        <f aca="false">ABS(C4-B4)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="F5" s="0" t="n">
+        <f aca="false">ABS(C5-B5)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="F6" s="0" t="n">
+        <f aca="false">ABS(C6-B6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="F7" s="0" t="n">
+        <f aca="false">ABS(C7-B7)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="F8" s="0" t="n">
+        <f aca="false">ABS(C8-B8)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="F9" s="0" t="n">
+        <f aca="false">ABS(C9-B9)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="6" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="F10" s="0" t="n">
+        <f aca="false">ABS(C10-B10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="F11" s="0" t="n">
+        <f aca="false">ABS(C11-B11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5" t="n">
+      <c r="B12" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="F12" s="0" t="n">
+        <f aca="false">ABS(C12-B12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="F13" s="0" t="n">
+        <f aca="false">ABS(C13-B13)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="6" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="F14" s="0" t="n">
+        <f aca="false">ABS(C14-B14)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="F15" s="0" t="n">
+        <f aca="false">ABS(C15-B15)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="F16" s="0" t="n">
+        <f aca="false">ABS(C16-B16)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="B17" s="5" t="n">
+      <c r="B17" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="F17" s="0" t="n">
+        <f aca="false">ABS(C17-B17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B18" s="5" t="n">
+      <c r="B18" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="F18" s="0" t="n">
+        <f aca="false">ABS(C18-B18)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B19" s="5" t="n">
+      <c r="B19" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="6" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="F19" s="0" t="n">
+        <f aca="false">ABS(C19-B19)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="B20" s="5" t="n">
+      <c r="B20" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="F20" s="0" t="n">
+        <f aca="false">ABS(C20-B20)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="B21" s="5" t="n">
+      <c r="B21" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="6" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="F21" s="0" t="n">
+        <f aca="false">ABS(C21-B21)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="n">
         <v>37</v>
       </c>
-      <c r="B22" s="5" t="n">
+      <c r="B22" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" s="6" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="F22" s="0" t="n">
+        <f aca="false">ABS(C22-B22)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="n">
         <v>38</v>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B23" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="F23" s="0" t="n">
+        <f aca="false">ABS(C23-B23)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="B24" s="5" t="n">
+      <c r="B24" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="F24" s="0" t="n">
+        <f aca="false">ABS(C24-B24)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B25" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" s="6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="F25" s="0" t="n">
+        <f aca="false">ABS(C25-B25)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
         <v>41</v>
       </c>
-      <c r="B26" s="5" t="n">
+      <c r="B26" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" s="6" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="F26" s="0" t="n">
+        <f aca="false">ABS(C26-B26)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
         <v>42</v>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B27" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="D27" s="6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="F27" s="0" t="n">
+        <f aca="false">ABS(C27-B27)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="F28" s="0" t="n">
+        <f aca="false">ABS(C28-B28)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B29" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="6" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="F29" s="0" t="n">
+        <f aca="false">ABS(C29-B29)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="B30" s="5" t="n">
+      <c r="B30" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="F30" s="0" t="n">
+        <f aca="false">ABS(C30-B30)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="B31" s="5" t="n">
+      <c r="B31" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C31" s="5" t="n">
+      <c r="C31" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="D31" s="6" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="F31" s="0" t="n">
+        <f aca="false">ABS(C31-B31)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="B32" s="5" t="n">
+      <c r="B32" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="C32" s="5" t="n">
+      <c r="C32" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="D32" s="6" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="F32" s="0" t="n">
+        <f aca="false">ABS(C32-B32)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="B33" s="5" t="n">
+      <c r="B33" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="C33" s="5" t="n">
+      <c r="C33" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="D33" s="6" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="F33" s="0" t="n">
+        <f aca="false">ABS(C33-B33)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="B34" s="5" t="n">
+      <c r="B34" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="C34" s="5" t="n">
+      <c r="C34" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="D34" s="5" t="n">
+      <c r="D34" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="F34" s="0" t="n">
+        <f aca="false">ABS(C34-B34)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="B35" s="5" t="n">
+      <c r="B35" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="C35" s="5" t="n">
+      <c r="C35" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="D35" s="5" t="n">
+      <c r="D35" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="F35" s="0" t="n">
+        <f aca="false">ABS(C35-B35)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
         <v>51</v>
       </c>
-      <c r="B36" s="5" t="n">
+      <c r="B36" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="D36" s="5" t="n">
+      <c r="D36" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="F36" s="0" t="n">
+        <f aca="false">ABS(C36-B36)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B37" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C37" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="D37" s="6" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="F37" s="0" t="n">
+        <f aca="false">ABS(C37-B37)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="n">
         <v>53</v>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B38" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="F38" s="0" t="n">
+        <f aca="false">ABS(C38-B38)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="B39" s="5" t="n">
+      <c r="B39" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C39" s="5" t="n">
+      <c r="C39" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D39" s="5" t="n">
+      <c r="D39" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="F39" s="0" t="n">
+        <f aca="false">ABS(C39-B39)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B40" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D40" s="6" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+      <c r="F40" s="0" t="n">
+        <f aca="false">ABS(C40-B40)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="n">
         <v>56</v>
       </c>
-      <c r="B41" s="5" t="n">
+      <c r="B41" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C41" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="D41" s="5" t="n">
+      <c r="D41" s="6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
+      <c r="F41" s="0" t="n">
+        <f aca="false">ABS(C41-B41)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="B42" s="5" t="n">
+      <c r="B42" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C42" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="D42" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
+      <c r="F42" s="0" t="n">
+        <f aca="false">ABS(C42-B42)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="n">
         <v>58</v>
       </c>
-      <c r="B43" s="5" t="n">
+      <c r="B43" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C43" s="5" t="n">
+      <c r="C43" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="D43" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
+      <c r="F43" s="0" t="n">
+        <f aca="false">ABS(C43-B43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="B44" s="5" t="n">
+      <c r="B44" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
+      <c r="F44" s="0" t="n">
+        <f aca="false">ABS(C44-B44)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="B45" s="5" t="n">
+      <c r="B45" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="D45" s="6" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
+      <c r="F45" s="0" t="n">
+        <f aca="false">ABS(C45-B45)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="n">
         <v>61</v>
       </c>
-      <c r="B46" s="5" t="n">
+      <c r="B46" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C46" s="5" t="n">
+      <c r="C46" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="D46" s="5" t="n">
+      <c r="D46" s="6" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+      <c r="F46" s="0" t="n">
+        <f aca="false">ABS(C46-B46)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="n">
         <v>62</v>
       </c>
-      <c r="B47" s="5" t="n">
+      <c r="B47" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="C47" s="5" t="n">
+      <c r="C47" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="D47" s="5" t="n">
+      <c r="D47" s="6" t="n">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+      <c r="F47" s="0" t="n">
+        <f aca="false">ABS(C47-B47)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="B48" s="5" t="n">
+      <c r="B48" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="D48" s="5" t="n">
+      <c r="D48" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
+      <c r="F48" s="0" t="n">
+        <f aca="false">ABS(C48-B48)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="B49" s="5" t="n">
+      <c r="B49" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="C49" s="5" t="n">
+      <c r="C49" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="D49" s="5" t="n">
+      <c r="D49" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
+      <c r="F49" s="0" t="n">
+        <f aca="false">ABS(C49-B49)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="B50" s="5" t="n">
+      <c r="B50" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="C50" s="5" t="n">
+      <c r="C50" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="D50" s="5" t="n">
+      <c r="D50" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="n">
+      <c r="F50" s="0" t="n">
+        <f aca="false">ABS(C50-B50)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="n">
         <v>66</v>
       </c>
-      <c r="B51" s="5" t="n">
+      <c r="B51" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C51" s="5" t="n">
+      <c r="C51" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D51" s="5" t="n">
+      <c r="D51" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
+      <c r="F51" s="0" t="n">
+        <f aca="false">ABS(C51-B51)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="B52" s="5" t="n">
+      <c r="B52" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C52" s="5" t="n">
+      <c r="C52" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="D52" s="5" t="n">
+      <c r="D52" s="6" t="n">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+      <c r="F52" s="0" t="n">
+        <f aca="false">ABS(C52-B52)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="n">
         <v>68</v>
       </c>
-      <c r="B53" s="5" t="n">
+      <c r="B53" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="D53" s="5" t="n">
+      <c r="D53" s="6" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
+      <c r="F53" s="0" t="n">
+        <f aca="false">ABS(C53-B53)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="n">
         <v>69</v>
       </c>
-      <c r="B54" s="5" t="n">
+      <c r="B54" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C54" s="5" t="n">
+      <c r="C54" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="D54" s="5" t="n">
+      <c r="D54" s="6" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
+      <c r="F54" s="0" t="n">
+        <f aca="false">ABS(C54-B54)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="B55" s="5" t="n">
+      <c r="B55" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C55" s="5" t="n">
+      <c r="C55" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D55" s="5" t="n">
+      <c r="D55" s="6" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
+      <c r="F55" s="0" t="n">
+        <f aca="false">ABS(C55-B55)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="n">
         <v>71</v>
       </c>
-      <c r="B56" s="5" t="n">
+      <c r="B56" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D56" s="6" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
+      <c r="F56" s="0" t="n">
+        <f aca="false">ABS(C56-B56)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="n">
         <v>72</v>
       </c>
-      <c r="B57" s="5" t="n">
+      <c r="B57" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="C57" s="5" t="n">
+      <c r="C57" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="D57" s="5" t="n">
+      <c r="D57" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
+      <c r="F57" s="0" t="n">
+        <f aca="false">ABS(C57-B57)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="B58" s="5" t="n">
+      <c r="B58" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="C58" s="5" t="n">
+      <c r="C58" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="D58" s="5" t="n">
+      <c r="D58" s="6" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
+      <c r="F58" s="0" t="n">
+        <f aca="false">ABS(C58-B58)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="B59" s="5" t="n">
+      <c r="B59" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="C59" s="5" t="n">
+      <c r="C59" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="D59" s="5" t="n">
+      <c r="D59" s="6" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
+      <c r="F59" s="0" t="n">
+        <f aca="false">ABS(C59-B59)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="B60" s="5" t="n">
+      <c r="B60" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C60" s="5" t="n">
+      <c r="C60" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D60" s="5" t="n">
+      <c r="D60" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
+      <c r="F60" s="0" t="n">
+        <f aca="false">ABS(C60-B60)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="B61" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C61" s="5" t="n">
+      <c r="B61" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="D61" s="5" t="n">
+      <c r="D61" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
+      <c r="F61" s="0" t="n">
+        <f aca="false">ABS(C61-B61)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="B62" s="5" t="n">
+      <c r="B62" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C62" s="5" t="n">
+      <c r="C62" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D62" s="5" t="n">
+      <c r="D62" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
+      <c r="F62" s="0" t="n">
+        <f aca="false">ABS(C62-B62)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="B63" s="5" t="n">
+      <c r="B63" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="C63" s="5" t="n">
+      <c r="C63" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="D63" s="5" t="n">
+      <c r="D63" s="6" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
+      <c r="F63" s="0" t="n">
+        <f aca="false">ABS(C63-B63)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="B64" s="5" t="n">
+      <c r="B64" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C64" s="5" t="n">
+      <c r="C64" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D64" s="5" t="n">
+      <c r="D64" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
+      <c r="F64" s="0" t="n">
+        <f aca="false">ABS(C64-B64)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="B65" s="5" t="n">
+      <c r="B65" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C65" s="5" t="n">
+      <c r="C65" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="D65" s="5" t="n">
+      <c r="D65" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
+      <c r="F65" s="0" t="n">
+        <f aca="false">ABS(C65-B65)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="B66" s="5" t="n">
+      <c r="B66" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C66" s="5" t="n">
+      <c r="C66" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="D66" s="5" t="n">
+      <c r="D66" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
+      <c r="F66" s="0" t="n">
+        <f aca="false">ABS(C66-B66)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="n">
         <v>78</v>
       </c>
-      <c r="B67" s="5" t="n">
+      <c r="B67" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="C67" s="5" t="n">
+      <c r="C67" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="D67" s="5" t="n">
+      <c r="D67" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="n">
+      <c r="F67" s="0" t="n">
+        <f aca="false">ABS(C67-B67)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="B68" s="5" t="n">
+      <c r="B68" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="C68" s="5" t="n">
+      <c r="C68" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="D68" s="5" t="n">
+      <c r="D68" s="6" t="n">
         <v>8</v>
       </c>
-    </row>
+      <c r="F68" s="0" t="n">
+        <f aca="false">ABS(C68-B68)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1628,28 +2016,28 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="7"/>
@@ -2504,4 +2892,966 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F79"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15" t="n">
+        <f aca="false">AVERAGE(A2:A68)</f>
+        <v>6.88059701492537</v>
+      </c>
+      <c r="B70" s="15" t="n">
+        <f aca="false">AVERAGE(B2:B68)</f>
+        <v>6.46268656716418</v>
+      </c>
+      <c r="C70" s="15" t="n">
+        <f aca="false">AVERAGE(C2:C68)</f>
+        <v>6.6865671641791</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="n">
+        <f aca="false">STDEV(A2:A68)</f>
+        <v>5.48419875659236</v>
+      </c>
+      <c r="B71" s="15" t="n">
+        <f aca="false">STDEV(B2:B68)</f>
+        <v>5.02818829415561</v>
+      </c>
+      <c r="C71" s="15" t="n">
+        <f aca="false">STDEV(C2:C68)</f>
+        <v>5.29782389638305</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E71" s="16"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="17" t="n">
+        <v>2145</v>
+      </c>
+      <c r="B72" s="17" t="n">
+        <v>2145</v>
+      </c>
+      <c r="C72" s="17" t="n">
+        <v>2080</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F72" s="19"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="20" t="n">
+        <v>1.17E-012</v>
+      </c>
+      <c r="B73" s="20" t="n">
+        <v>1.172E-012</v>
+      </c>
+      <c r="C73" s="20" t="n">
+        <v>1.711E-012</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F73" s="19"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="21" t="n">
+        <v>2145</v>
+      </c>
+      <c r="B75" s="21" t="n">
+        <v>2145</v>
+      </c>
+      <c r="C75" s="22" t="n">
+        <v>2080</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B76" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A79:E79"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>